<commit_message>
Added Docker installation instructions
</commit_message>
<xml_diff>
--- a/Degraders_list.xlsx
+++ b/Degraders_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="435">
   <si>
     <t xml:space="preserve">Microorganism</t>
   </si>
@@ -1168,7 +1168,7 @@
     <t xml:space="preserve">Amycolatopsis sp.</t>
   </si>
   <si>
-    <t xml:space="preserve">Emadian, S. M., Onay, T. T., &amp; Demirel, B. (2017). Biodegradation of bioplastics in natural environments. Waste management, 59, 526-536.</t>
+    <t xml:space="preserve">Teeraphatpornchai, T., Nakajima-Kambe, T., Shigeno-Akutsu, Y., Nakayama, M., Nomura, N., Nakahara, T., &amp; Uchiyama, H. (2003). Isolation and characterization of a bacterium that degrades various polyester-based biodegradable plastics. Biotechnology letters, 25(1), 23-28., Sukkhum, S., Tokuyama, S., Tamura, T., &amp; Kitpreechavanich, V. (2009). A novel poly (L-lactide) degrading actinomycetes isolated from Thai forest soil, phylogenic relationship and the enzyme characterization. The Journal of general and applied microbiology, 55(6), 459-467., Kim, M. N., &amp; Park, S. T. (2010). Degradation of poly (L‐lactide) by a mesophilic bacterium. Journal of applied polymer science, 117(1), 67-74., A. Chomchoei, W. Pathom-Aree, A. Yokota, C. Kanongnuch, S. Lumyong Amycolatopsis thailandensis sp. nov., a poly(l-lactic acid)-degrading actinomycete, isolated from soil Int. J. Syst. Evol. Microbiol., 61 (2011), pp. 839-843, Penkhrue, W., Khanongnuch, C., Masaki, K., Pathom-aree, W., Punyodom, W., &amp; Lumyong, S. (2015). Isolation and screening of biopolymer-degrading microorganisms from northern Thailand. [World Journal of Microbiology and Biotechnology, 31(9), 1431-1442.] via Emadian, S. M., Onay, T. T., &amp; Demirel, B. (2017). Biodegradation of bioplastics in natural environments. Waste management, 59, 526-536.</t>
   </si>
   <si>
     <t xml:space="preserve">Amycolatopsis thailandensis</t>
@@ -1448,8 +1448,8 @@
   </sheetPr>
   <dimension ref="A1:F490"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A380" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A381" activeCellId="0" sqref="A381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9072,9 +9072,6 @@
       <c r="C381" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D381" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E381" s="2" t="s">
         <v>9</v>
       </c>
@@ -9092,9 +9089,6 @@
       <c r="C382" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D382" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E382" s="2" t="s">
         <v>9</v>
       </c>
@@ -9112,9 +9106,6 @@
       <c r="C383" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D383" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E383" s="2" t="s">
         <v>9</v>
       </c>
@@ -9132,9 +9123,6 @@
       <c r="C384" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D384" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E384" s="2" t="s">
         <v>9</v>
       </c>
@@ -9152,9 +9140,6 @@
       <c r="C385" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D385" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E385" s="2" t="s">
         <v>9</v>
       </c>
@@ -9172,9 +9157,6 @@
       <c r="C386" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D386" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E386" s="2" t="s">
         <v>9</v>
       </c>
@@ -9192,9 +9174,6 @@
       <c r="C387" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D387" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E387" s="2" t="s">
         <v>9</v>
       </c>
@@ -9212,9 +9191,6 @@
       <c r="C388" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D388" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E388" s="2" t="s">
         <v>9</v>
       </c>
@@ -9232,9 +9208,6 @@
       <c r="C389" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D389" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E389" s="2" t="s">
         <v>9</v>
       </c>
@@ -9252,9 +9225,6 @@
       <c r="C390" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D390" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E390" s="2" t="s">
         <v>9</v>
       </c>
@@ -9272,9 +9242,6 @@
       <c r="C391" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D391" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E391" s="2" t="s">
         <v>9</v>
       </c>
@@ -9292,9 +9259,6 @@
       <c r="C392" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D392" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E392" s="2" t="s">
         <v>9</v>
       </c>
@@ -9312,9 +9276,6 @@
       <c r="C393" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D393" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E393" s="2" t="s">
         <v>9</v>
       </c>
@@ -9332,9 +9293,6 @@
       <c r="C394" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D394" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E394" s="2" t="s">
         <v>9</v>
       </c>
@@ -9352,9 +9310,6 @@
       <c r="C395" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D395" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E395" s="2" t="s">
         <v>9</v>
       </c>
@@ -9372,9 +9327,6 @@
       <c r="C396" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D396" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E396" s="2" t="s">
         <v>9</v>
       </c>
@@ -9392,9 +9344,6 @@
       <c r="C397" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D397" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E397" s="2" t="s">
         <v>9</v>
       </c>
@@ -9412,9 +9361,6 @@
       <c r="C398" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D398" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E398" s="2" t="s">
         <v>9</v>
       </c>
@@ -9432,9 +9378,6 @@
       <c r="C399" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D399" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E399" s="2" t="s">
         <v>9</v>
       </c>
@@ -9452,9 +9395,6 @@
       <c r="C400" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D400" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E400" s="2" t="s">
         <v>9</v>
       </c>
@@ -9472,9 +9412,6 @@
       <c r="C401" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D401" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E401" s="2" t="s">
         <v>9</v>
       </c>
@@ -9492,9 +9429,6 @@
       <c r="C402" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D402" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E402" s="2" t="s">
         <v>9</v>
       </c>
@@ -9512,9 +9446,6 @@
       <c r="C403" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="D403" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E403" s="2" t="s">
         <v>9</v>
       </c>
@@ -9532,9 +9463,6 @@
       <c r="C404" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D404" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E404" s="2" t="s">
         <v>9</v>
       </c>
@@ -9552,9 +9480,6 @@
       <c r="C405" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D405" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E405" s="2" t="s">
         <v>9</v>
       </c>
@@ -9572,9 +9497,6 @@
       <c r="C406" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D406" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E406" s="2" t="s">
         <v>9</v>
       </c>
@@ -9592,9 +9514,6 @@
       <c r="C407" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D407" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E407" s="2" t="s">
         <v>9</v>
       </c>
@@ -9612,9 +9531,6 @@
       <c r="C408" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D408" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E408" s="2" t="s">
         <v>9</v>
       </c>
@@ -9632,9 +9548,6 @@
       <c r="C409" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D409" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E409" s="2" t="s">
         <v>9</v>
       </c>
@@ -9652,9 +9565,6 @@
       <c r="C410" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D410" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E410" s="2" t="s">
         <v>9</v>
       </c>
@@ -9672,9 +9582,6 @@
       <c r="C411" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D411" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E411" s="2" t="s">
         <v>9</v>
       </c>
@@ -9692,9 +9599,6 @@
       <c r="C412" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D412" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E412" s="2" t="s">
         <v>9</v>
       </c>
@@ -9712,9 +9616,6 @@
       <c r="C413" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D413" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E413" s="2" t="s">
         <v>9</v>
       </c>
@@ -9732,9 +9633,6 @@
       <c r="C414" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D414" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E414" s="2" t="s">
         <v>9</v>
       </c>
@@ -9752,9 +9650,6 @@
       <c r="C415" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D415" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E415" s="2" t="s">
         <v>9</v>
       </c>
@@ -9772,9 +9667,6 @@
       <c r="C416" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D416" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E416" s="2" t="s">
         <v>9</v>
       </c>
@@ -9792,9 +9684,6 @@
       <c r="C417" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D417" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E417" s="2" t="s">
         <v>9</v>
       </c>
@@ -9812,9 +9701,6 @@
       <c r="C418" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D418" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E418" s="2" t="s">
         <v>9</v>
       </c>
@@ -9832,9 +9718,6 @@
       <c r="C419" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D419" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E419" s="2" t="s">
         <v>9</v>
       </c>
@@ -9852,9 +9735,6 @@
       <c r="C420" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D420" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E420" s="2" t="s">
         <v>9</v>
       </c>
@@ -9872,9 +9752,6 @@
       <c r="C421" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D421" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E421" s="2" t="s">
         <v>9</v>
       </c>
@@ -9892,9 +9769,6 @@
       <c r="C422" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D422" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E422" s="2" t="s">
         <v>9</v>
       </c>
@@ -9912,9 +9786,6 @@
       <c r="C423" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D423" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E423" s="2" t="s">
         <v>9</v>
       </c>
@@ -9932,9 +9803,6 @@
       <c r="C424" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D424" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E424" s="2" t="s">
         <v>9</v>
       </c>
@@ -9952,9 +9820,6 @@
       <c r="C425" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D425" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E425" s="2" t="s">
         <v>9</v>
       </c>
@@ -9972,9 +9837,6 @@
       <c r="C426" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D426" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E426" s="2" t="s">
         <v>9</v>
       </c>
@@ -9992,9 +9854,6 @@
       <c r="C427" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D427" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E427" s="2" t="s">
         <v>9</v>
       </c>
@@ -10012,9 +9871,6 @@
       <c r="C428" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D428" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E428" s="2" t="s">
         <v>9</v>
       </c>
@@ -10032,9 +9888,6 @@
       <c r="C429" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D429" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E429" s="2" t="s">
         <v>9</v>
       </c>
@@ -10052,9 +9905,6 @@
       <c r="C430" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D430" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E430" s="2" t="s">
         <v>9</v>
       </c>
@@ -10072,9 +9922,6 @@
       <c r="C431" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D431" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E431" s="2" t="s">
         <v>9</v>
       </c>
@@ -10092,9 +9939,6 @@
       <c r="C432" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D432" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E432" s="2" t="s">
         <v>9</v>
       </c>
@@ -10112,9 +9956,6 @@
       <c r="C433" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D433" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E433" s="2" t="s">
         <v>9</v>
       </c>
@@ -10132,9 +9973,6 @@
       <c r="C434" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D434" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E434" s="2" t="s">
         <v>9</v>
       </c>
@@ -10152,9 +9990,6 @@
       <c r="C435" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D435" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E435" s="2" t="s">
         <v>9</v>
       </c>
@@ -10172,9 +10007,6 @@
       <c r="C436" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D436" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E436" s="2" t="s">
         <v>9</v>
       </c>
@@ -10192,9 +10024,6 @@
       <c r="C437" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D437" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E437" s="2" t="s">
         <v>9</v>
       </c>
@@ -10212,9 +10041,6 @@
       <c r="C438" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D438" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E438" s="2" t="s">
         <v>9</v>
       </c>
@@ -10232,9 +10058,6 @@
       <c r="C439" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D439" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E439" s="2" t="s">
         <v>9</v>
       </c>
@@ -10252,9 +10075,6 @@
       <c r="C440" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="D440" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E440" s="2" t="s">
         <v>9</v>
       </c>
@@ -10272,9 +10092,6 @@
       <c r="C441" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D441" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E441" s="2" t="s">
         <v>9</v>
       </c>
@@ -10292,9 +10109,6 @@
       <c r="C442" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D442" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E442" s="2" t="s">
         <v>9</v>
       </c>
@@ -10312,9 +10126,6 @@
       <c r="C443" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D443" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E443" s="2" t="s">
         <v>9</v>
       </c>
@@ -10332,9 +10143,6 @@
       <c r="C444" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D444" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E444" s="2" t="s">
         <v>9</v>
       </c>
@@ -10352,9 +10160,6 @@
       <c r="C445" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D445" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E445" s="2" t="s">
         <v>9</v>
       </c>
@@ -10372,9 +10177,6 @@
       <c r="C446" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D446" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E446" s="2" t="s">
         <v>9</v>
       </c>
@@ -10392,9 +10194,6 @@
       <c r="C447" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D447" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E447" s="2" t="s">
         <v>9</v>
       </c>
@@ -10412,9 +10211,6 @@
       <c r="C448" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D448" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E448" s="2" t="s">
         <v>9</v>
       </c>
@@ -10432,9 +10228,6 @@
       <c r="C449" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D449" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E449" s="2" t="s">
         <v>9</v>
       </c>
@@ -10452,9 +10245,6 @@
       <c r="C450" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D450" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E450" s="2" t="s">
         <v>9</v>
       </c>
@@ -10472,9 +10262,6 @@
       <c r="C451" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D451" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E451" s="2" t="s">
         <v>9</v>
       </c>
@@ -10492,9 +10279,6 @@
       <c r="C452" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D452" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E452" s="2" t="s">
         <v>9</v>
       </c>
@@ -10512,9 +10296,6 @@
       <c r="C453" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D453" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E453" s="2" t="s">
         <v>9</v>
       </c>
@@ -10532,9 +10313,6 @@
       <c r="C454" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D454" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E454" s="2" t="s">
         <v>9</v>
       </c>
@@ -10552,9 +10330,6 @@
       <c r="C455" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D455" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E455" s="2" t="s">
         <v>9</v>
       </c>
@@ -10572,9 +10347,6 @@
       <c r="C456" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D456" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E456" s="2" t="s">
         <v>9</v>
       </c>
@@ -10592,9 +10364,6 @@
       <c r="C457" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D457" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E457" s="2" t="s">
         <v>9</v>
       </c>
@@ -10612,9 +10381,6 @@
       <c r="C458" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D458" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E458" s="2" t="s">
         <v>9</v>
       </c>
@@ -10632,9 +10398,6 @@
       <c r="C459" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D459" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E459" s="2" t="s">
         <v>9</v>
       </c>
@@ -10652,9 +10415,6 @@
       <c r="C460" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D460" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E460" s="2" t="s">
         <v>9</v>
       </c>
@@ -10672,9 +10432,6 @@
       <c r="C461" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D461" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E461" s="2" t="s">
         <v>9</v>
       </c>
@@ -10692,9 +10449,6 @@
       <c r="C462" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D462" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E462" s="2" t="s">
         <v>9</v>
       </c>
@@ -10712,9 +10466,6 @@
       <c r="C463" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D463" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E463" s="2" t="s">
         <v>9</v>
       </c>
@@ -10732,9 +10483,6 @@
       <c r="C464" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D464" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E464" s="2" t="s">
         <v>9</v>
       </c>
@@ -10752,9 +10500,6 @@
       <c r="C465" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D465" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E465" s="2" t="s">
         <v>9</v>
       </c>
@@ -10772,9 +10517,6 @@
       <c r="C466" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D466" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E466" s="2" t="s">
         <v>9</v>
       </c>
@@ -10792,9 +10534,6 @@
       <c r="C467" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D467" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E467" s="2" t="s">
         <v>9</v>
       </c>
@@ -10812,9 +10551,6 @@
       <c r="C468" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D468" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E468" s="2" t="s">
         <v>9</v>
       </c>
@@ -10832,9 +10568,6 @@
       <c r="C469" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D469" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E469" s="2" t="s">
         <v>9</v>
       </c>
@@ -10852,9 +10585,6 @@
       <c r="C470" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D470" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E470" s="2" t="s">
         <v>9</v>
       </c>
@@ -10872,9 +10602,6 @@
       <c r="C471" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D471" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E471" s="2" t="s">
         <v>9</v>
       </c>
@@ -10892,9 +10619,6 @@
       <c r="C472" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D472" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E472" s="2" t="s">
         <v>9</v>
       </c>
@@ -10912,9 +10636,6 @@
       <c r="C473" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D473" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E473" s="2" t="s">
         <v>9</v>
       </c>
@@ -10932,9 +10653,6 @@
       <c r="C474" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D474" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E474" s="2" t="s">
         <v>9</v>
       </c>
@@ -10952,9 +10670,6 @@
       <c r="C475" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D475" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E475" s="2" t="s">
         <v>9</v>
       </c>
@@ -10972,9 +10687,6 @@
       <c r="C476" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D476" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E476" s="2" t="s">
         <v>9</v>
       </c>
@@ -10992,9 +10704,6 @@
       <c r="C477" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D477" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E477" s="2" t="s">
         <v>9</v>
       </c>
@@ -11012,9 +10721,6 @@
       <c r="C478" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D478" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E478" s="2" t="s">
         <v>9</v>
       </c>
@@ -11032,9 +10738,6 @@
       <c r="C479" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D479" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E479" s="2" t="s">
         <v>9</v>
       </c>
@@ -11052,9 +10755,6 @@
       <c r="C480" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D480" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E480" s="2" t="s">
         <v>9</v>
       </c>
@@ -11072,9 +10772,6 @@
       <c r="C481" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D481" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E481" s="2" t="s">
         <v>9</v>
       </c>
@@ -11092,9 +10789,6 @@
       <c r="C482" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D482" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E482" s="2" t="s">
         <v>9</v>
       </c>
@@ -11112,9 +10806,6 @@
       <c r="C483" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D483" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E483" s="2" t="s">
         <v>9</v>
       </c>
@@ -11132,9 +10823,6 @@
       <c r="C484" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D484" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E484" s="2" t="s">
         <v>9</v>
       </c>
@@ -11152,9 +10840,6 @@
       <c r="C485" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D485" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E485" s="2" t="s">
         <v>9</v>
       </c>
@@ -11172,9 +10857,6 @@
       <c r="C486" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D486" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E486" s="2" t="s">
         <v>9</v>
       </c>
@@ -11192,9 +10874,6 @@
       <c r="C487" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D487" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E487" s="2" t="s">
         <v>9</v>
       </c>
@@ -11212,9 +10891,6 @@
       <c r="C488" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D488" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="E488" s="2" t="s">
         <v>9</v>
       </c>
@@ -11231,9 +10907,6 @@
       </c>
       <c r="C489" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D489" s="0" t="s">
-        <v>382</v>
       </c>
       <c r="E489" s="2" t="s">
         <v>9</v>

</xml_diff>